<commit_message>
add gantt in projrct plan
</commit_message>
<xml_diff>
--- a/resources/matrix.xlsx
+++ b/resources/matrix.xlsx
@@ -8,17 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AAAAAAAAcourse\T2\soft-tech\A1\SoftwareTechnologyGroup47\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7DA3B68-460A-46DB-8300-16BBA27BE9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B54E7DE-8310-4A6C-8D9B-8DE673B0C89E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>

</xml_diff>